<commit_message>
Extracted and added dimension tables
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://afzdxb-my.sharepoint.com/personal/innocent_kyalo_alfazance_com/Documents/Desktop/BI/NYC Trips/NYC Trips/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\PowerBI Projects\NYC Trips Project\NYC-Trips-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{1AA33C61-4EFF-43BD-B50C-2F0E6F368152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{861FDAF9-FA3C-4AF6-B2C1-45C436B57DE1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD8FA6C-081B-4B8C-91AF-7371BEB441DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9A053699-A66A-4C45-B4DF-767E187D10B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A053699-A66A-4C45-B4DF-767E187D10B9}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
   <si>
     <t>Field</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +481,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -638,9 +656,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -705,17 +731,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA96E775-6C3B-4DCE-920F-1CE4AEE1C5A1}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20" xr:uid="{DA96E775-6C3B-4DCE-920F-1CE4AEE1C5A1}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA96E775-6C3B-4DCE-920F-1CE4AEE1C5A1}" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0">
+  <autoFilter ref="A1:D20" xr:uid="{DA96E775-6C3B-4DCE-920F-1CE4AEE1C5A1}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E57DE6CB-C291-45D9-A8FF-4B9B2D090972}" name="Field"/>
     <tableColumn id="2" xr3:uid="{CC6A9EF5-65C4-4C8A-8A5D-5955C587A29C}" name="Description" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{01DEC5B8-DEA6-406C-B4B3-890F32F0C19A}" name="Data Type"/>
+    <tableColumn id="4" xr3:uid="{CB34B3F7-4106-412B-B40B-AF5E824821F8}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1038,21 +1061,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC98B23-9665-4A4B-8EB8-E5A8C8A15CBA}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C21" sqref="C21"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" customWidth="1"/>
-    <col min="2" max="2" width="79.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="79.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1062,85 +1086,109 @@
       <c r="C1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1150,8 +1198,11 @@
       <c r="C9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1161,8 +1212,11 @@
       <c r="C10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1172,104 +1226,134 @@
       <c r="C11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="C19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>